<commit_message>
only logs from ofc
</commit_message>
<xml_diff>
--- a/strategy/pnl/Index_Option_Writing_PnL.xlsx
+++ b/strategy/pnl/Index_Option_Writing_PnL.xlsx
@@ -10,6 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="08-03-2021" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="12-03-2021" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="15-03-2021" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="17-03-2021" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" iterateDelta="0.0001"/>
@@ -7071,7 +7072,7 @@
     </row>
     <row r="7">
       <c r="A7" s="6" t="n">
-        <v>44270.41944444444</v>
+        <v>44270.41944444443</v>
       </c>
       <c r="B7" t="n">
         <v>-682.5</v>
@@ -7268,7 +7269,7 @@
     </row>
     <row r="14">
       <c r="A14" s="6" t="n">
-        <v>44270.42430555556</v>
+        <v>44270.42430555557</v>
       </c>
       <c r="B14" t="n">
         <v>-142.5</v>
@@ -8099,7 +8100,7 @@
     </row>
     <row r="27">
       <c r="A27" s="6" t="n">
-        <v>44270.43333333333</v>
+        <v>44270.43333333332</v>
       </c>
       <c r="B27" t="n">
         <v>-1842.5</v>
@@ -8303,7 +8304,7 @@
     </row>
     <row r="39">
       <c r="A39" s="6" t="n">
-        <v>44270.44166666667</v>
+        <v>44270.44166666668</v>
       </c>
       <c r="B39" t="n">
         <v>-460</v>
@@ -8524,7 +8525,7 @@
     </row>
     <row r="52">
       <c r="A52" s="6" t="n">
-        <v>44270.45069444444</v>
+        <v>44270.45069444443</v>
       </c>
       <c r="B52" t="n">
         <v>-328.75</v>
@@ -8643,7 +8644,7 @@
     </row>
     <row r="59">
       <c r="A59" s="6" t="n">
-        <v>44270.45555555556</v>
+        <v>44270.45555555557</v>
       </c>
       <c r="B59" t="n">
         <v>1306.25</v>
@@ -8864,7 +8865,7 @@
     </row>
     <row r="72">
       <c r="A72" s="6" t="n">
-        <v>44270.46458333333</v>
+        <v>44270.46458333332</v>
       </c>
       <c r="B72" t="n">
         <v>3583.75</v>
@@ -9068,7 +9069,7 @@
     </row>
     <row r="84">
       <c r="A84" s="6" t="n">
-        <v>44270.47291666667</v>
+        <v>44270.47291666668</v>
       </c>
       <c r="B84" t="n">
         <v>5111.25</v>
@@ -9289,7 +9290,7 @@
     </row>
     <row r="97">
       <c r="A97" s="6" t="n">
-        <v>44270.48194444444</v>
+        <v>44270.48194444443</v>
       </c>
       <c r="B97" t="n">
         <v>3880</v>
@@ -9408,7 +9409,7 @@
     </row>
     <row r="104">
       <c r="A104" s="6" t="n">
-        <v>44270.48680555556</v>
+        <v>44270.48680555557</v>
       </c>
       <c r="B104" t="n">
         <v>3936.25</v>
@@ -9629,7 +9630,7 @@
     </row>
     <row r="117">
       <c r="A117" s="6" t="n">
-        <v>44270.49583333333</v>
+        <v>44270.49583333332</v>
       </c>
       <c r="B117" t="n">
         <v>4787.5</v>
@@ -9833,7 +9834,7 @@
     </row>
     <row r="129">
       <c r="A129" s="6" t="n">
-        <v>44270.50416666667</v>
+        <v>44270.50416666668</v>
       </c>
       <c r="B129" t="n">
         <v>3186.25</v>
@@ -10054,7 +10055,7 @@
     </row>
     <row r="142">
       <c r="A142" s="6" t="n">
-        <v>44270.51319444444</v>
+        <v>44270.51319444443</v>
       </c>
       <c r="B142" t="n">
         <v>4730</v>
@@ -10173,7 +10174,7 @@
     </row>
     <row r="149">
       <c r="A149" s="6" t="n">
-        <v>44270.51805555556</v>
+        <v>44270.51805555557</v>
       </c>
       <c r="B149" t="n">
         <v>4740</v>
@@ -10394,7 +10395,7 @@
     </row>
     <row r="162">
       <c r="A162" s="6" t="n">
-        <v>44270.52708333333</v>
+        <v>44270.52708333332</v>
       </c>
       <c r="B162" t="n">
         <v>6246.25</v>
@@ -10598,7 +10599,7 @@
     </row>
     <row r="174">
       <c r="A174" s="6" t="n">
-        <v>44270.53541666667</v>
+        <v>44270.53541666668</v>
       </c>
       <c r="B174" t="n">
         <v>4990</v>
@@ -10819,7 +10820,7 @@
     </row>
     <row r="187">
       <c r="A187" s="6" t="n">
-        <v>44270.54444444444</v>
+        <v>44270.54444444443</v>
       </c>
       <c r="B187" t="n">
         <v>6401.25</v>
@@ -10938,7 +10939,7 @@
     </row>
     <row r="194">
       <c r="A194" s="6" t="n">
-        <v>44270.54930555556</v>
+        <v>44270.54930555557</v>
       </c>
       <c r="B194" t="n">
         <v>6307.5</v>
@@ -11159,7 +11160,7 @@
     </row>
     <row r="207">
       <c r="A207" s="6" t="n">
-        <v>44270.55833333333</v>
+        <v>44270.55833333332</v>
       </c>
       <c r="B207" t="n">
         <v>5250</v>
@@ -11363,7 +11364,7 @@
     </row>
     <row r="219">
       <c r="A219" s="6" t="n">
-        <v>44270.56666666667</v>
+        <v>44270.56666666668</v>
       </c>
       <c r="B219" t="n">
         <v>4396.25</v>
@@ -11584,7 +11585,7 @@
     </row>
     <row r="232">
       <c r="A232" s="6" t="n">
-        <v>44270.57569444444</v>
+        <v>44270.57569444443</v>
       </c>
       <c r="B232" t="n">
         <v>3552.5</v>
@@ -11703,7 +11704,7 @@
     </row>
     <row r="239">
       <c r="A239" s="6" t="n">
-        <v>44270.58055555556</v>
+        <v>44270.58055555557</v>
       </c>
       <c r="B239" t="n">
         <v>2290</v>
@@ -11924,7 +11925,7 @@
     </row>
     <row r="252">
       <c r="A252" s="6" t="n">
-        <v>44270.58958333333</v>
+        <v>44270.58958333332</v>
       </c>
       <c r="B252" t="n">
         <v>5346.25</v>
@@ -12128,7 +12129,7 @@
     </row>
     <row r="264">
       <c r="A264" s="6" t="n">
-        <v>44270.59791666667</v>
+        <v>44270.59791666668</v>
       </c>
       <c r="B264" t="n">
         <v>4066.25</v>
@@ -12349,7 +12350,7 @@
     </row>
     <row r="277">
       <c r="A277" s="6" t="n">
-        <v>44270.60694444444</v>
+        <v>44270.60694444443</v>
       </c>
       <c r="B277" t="n">
         <v>3187.5</v>
@@ -12468,7 +12469,7 @@
     </row>
     <row r="284">
       <c r="A284" s="6" t="n">
-        <v>44270.61180555556</v>
+        <v>44270.61180555557</v>
       </c>
       <c r="B284" t="n">
         <v>71.25</v>
@@ -12689,7 +12690,7 @@
     </row>
     <row r="297">
       <c r="A297" s="6" t="n">
-        <v>44270.62083333333</v>
+        <v>44270.62083333332</v>
       </c>
       <c r="B297" t="n">
         <v>477.5</v>
@@ -12753,6 +12754,3532 @@
       </c>
       <c r="E300" t="n">
         <v>-2638.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U163"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>open</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>high</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>close</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>MaxPnL</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>MinPnL</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>FinalPnL</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="n">
+        <v>44272.41597222222</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>31.25</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-92.5</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-92.5</v>
+      </c>
+      <c r="G2">
+        <f>MAX(E:E)</f>
+        <v/>
+      </c>
+      <c r="H2">
+        <f>MIN(E:E)</f>
+        <v/>
+      </c>
+      <c r="I2" t="n">
+        <v>-3137.5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="n">
+        <v>44272.41666666666</v>
+      </c>
+      <c r="B3" t="n">
+        <v>42.5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>206.25</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-7.5</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-7.5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="n">
+        <v>44272.41736111111</v>
+      </c>
+      <c r="B4" t="n">
+        <v>95</v>
+      </c>
+      <c r="C4" t="n">
+        <v>205</v>
+      </c>
+      <c r="D4" t="n">
+        <v>95</v>
+      </c>
+      <c r="E4" t="n">
+        <v>166.25</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="n">
+        <v>44272.41805555556</v>
+      </c>
+      <c r="B5" t="n">
+        <v>166.25</v>
+      </c>
+      <c r="C5" t="n">
+        <v>166.25</v>
+      </c>
+      <c r="D5" t="n">
+        <v>107.5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>107.5</v>
+      </c>
+      <c r="H5" s="4" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="I5" s="4" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="J5" s="4" t="inlineStr">
+        <is>
+          <t>tr_qty</t>
+        </is>
+      </c>
+      <c r="K5" s="4" t="inlineStr">
+        <is>
+          <t>tradedPrice</t>
+        </is>
+      </c>
+      <c r="L5" s="4" t="inlineStr">
+        <is>
+          <t>tr_amount</t>
+        </is>
+      </c>
+      <c r="M5" s="4" t="inlineStr">
+        <is>
+          <t>ltp</t>
+        </is>
+      </c>
+      <c r="N5" s="4" t="inlineStr">
+        <is>
+          <t>cur_amount</t>
+        </is>
+      </c>
+      <c r="O5" s="4" t="inlineStr">
+        <is>
+          <t>pnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="6" t="n">
+        <v>44272.41875</v>
+      </c>
+      <c r="B6" t="n">
+        <v>33.75</v>
+      </c>
+      <c r="C6" t="n">
+        <v>145</v>
+      </c>
+      <c r="D6" t="n">
+        <v>33.75</v>
+      </c>
+      <c r="E6" t="n">
+        <v>117.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>55197</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>BANKNIFTY2131834600PE</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>561.35</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-733.7500000000009</v>
+      </c>
+      <c r="M6" t="n">
+        <v>265.25</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>733.7500000000009</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="6" t="n">
+        <v>44272.41944444444</v>
+      </c>
+      <c r="B7" t="n">
+        <v>103.75</v>
+      </c>
+      <c r="C7" t="n">
+        <v>103.75</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-46.25</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-46.25</v>
+      </c>
+      <c r="H7" t="n">
+        <v>55245</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>BANKNIFTY2131834800CE</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>642</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1542.500000000001</v>
+      </c>
+      <c r="M7" t="n">
+        <v>266.7</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>-1542.500000000001</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="6" t="n">
+        <v>44272.42013888889</v>
+      </c>
+      <c r="B8" t="n">
+        <v>-46.25</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-46.25</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-46.25</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-46.25</v>
+      </c>
+      <c r="H8" t="n">
+        <v>56445</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>NIFTY2131814850PE</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>164.35</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1166.25</v>
+      </c>
+      <c r="M8" t="n">
+        <v>88.59999999999999</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-1166.25</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="6" t="n">
+        <v>44272.42083333333</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-46.25</v>
+      </c>
+      <c r="C9" t="n">
+        <v>152.5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-46.25</v>
+      </c>
+      <c r="E9" t="n">
+        <v>151.25</v>
+      </c>
+      <c r="H9" t="n">
+        <v>56448</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>NIFTY2131814950CE</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>161.4</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1162.5</v>
+      </c>
+      <c r="M9" t="n">
+        <v>46.6</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>-1162.5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="n">
+        <v>44272.42152777778</v>
+      </c>
+      <c r="B10" t="n">
+        <v>311.25</v>
+      </c>
+      <c r="C10" t="n">
+        <v>311.25</v>
+      </c>
+      <c r="D10" t="n">
+        <v>161.25</v>
+      </c>
+      <c r="E10" t="n">
+        <v>278.75</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="n">
+        <v>44272.42222222222</v>
+      </c>
+      <c r="B11" t="n">
+        <v>198.75</v>
+      </c>
+      <c r="C11" t="n">
+        <v>330</v>
+      </c>
+      <c r="D11" t="n">
+        <v>198.75</v>
+      </c>
+      <c r="E11" t="n">
+        <v>277.5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="n">
+        <v>44272.42291666667</v>
+      </c>
+      <c r="B12" t="n">
+        <v>291.25</v>
+      </c>
+      <c r="C12" t="n">
+        <v>318.75</v>
+      </c>
+      <c r="D12" t="n">
+        <v>248.75</v>
+      </c>
+      <c r="E12" t="n">
+        <v>248.75</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="n">
+        <v>44272.42361111111</v>
+      </c>
+      <c r="B13" t="n">
+        <v>248.75</v>
+      </c>
+      <c r="C13" t="n">
+        <v>411.25</v>
+      </c>
+      <c r="D13" t="n">
+        <v>248.75</v>
+      </c>
+      <c r="E13" t="n">
+        <v>411.25</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="n">
+        <v>44272.42430555556</v>
+      </c>
+      <c r="B14" t="n">
+        <v>411.25</v>
+      </c>
+      <c r="C14" t="n">
+        <v>558.75</v>
+      </c>
+      <c r="D14" t="n">
+        <v>411.25</v>
+      </c>
+      <c r="E14" t="n">
+        <v>508.75</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="n">
+        <v>44272.425</v>
+      </c>
+      <c r="B15" t="n">
+        <v>571.25</v>
+      </c>
+      <c r="C15" t="n">
+        <v>571.25</v>
+      </c>
+      <c r="D15" t="n">
+        <v>525</v>
+      </c>
+      <c r="E15" t="n">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6" t="n">
+        <v>44272.42569444444</v>
+      </c>
+      <c r="B16" t="n">
+        <v>455</v>
+      </c>
+      <c r="C16" t="n">
+        <v>455</v>
+      </c>
+      <c r="D16" t="n">
+        <v>386.25</v>
+      </c>
+      <c r="E16" t="n">
+        <v>386.25</v>
+      </c>
+      <c r="H16" s="4" t="inlineStr">
+        <is>
+          <t>set</t>
+        </is>
+      </c>
+      <c r="I16" s="4" t="inlineStr">
+        <is>
+          <t>txn_type</t>
+        </is>
+      </c>
+      <c r="J16" s="4" t="inlineStr">
+        <is>
+          <t>strike</t>
+        </is>
+      </c>
+      <c r="K16" s="4" t="inlineStr">
+        <is>
+          <t>qty</t>
+        </is>
+      </c>
+      <c r="L16" s="4" t="inlineStr">
+        <is>
+          <t>tr_qty</t>
+        </is>
+      </c>
+      <c r="M16" s="4" t="inlineStr">
+        <is>
+          <t>expiry</t>
+        </is>
+      </c>
+      <c r="N16" s="4" t="inlineStr">
+        <is>
+          <t>optionType</t>
+        </is>
+      </c>
+      <c r="O16" s="4" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="P16" s="4" t="inlineStr">
+        <is>
+          <t>symbol</t>
+        </is>
+      </c>
+      <c r="Q16" s="4" t="inlineStr">
+        <is>
+          <t>orderID</t>
+        </is>
+      </c>
+      <c r="R16" s="4" t="inlineStr">
+        <is>
+          <t>tradedPrice</t>
+        </is>
+      </c>
+      <c r="S16" s="4" t="inlineStr">
+        <is>
+          <t>dateTime</t>
+        </is>
+      </c>
+      <c r="T16" s="4" t="inlineStr">
+        <is>
+          <t>set_type</t>
+        </is>
+      </c>
+      <c r="U16" s="4" t="inlineStr">
+        <is>
+          <t>tr_amount</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6" t="n">
+        <v>44272.42638888889</v>
+      </c>
+      <c r="B17" t="n">
+        <v>425</v>
+      </c>
+      <c r="C17" t="n">
+        <v>425</v>
+      </c>
+      <c r="D17" t="n">
+        <v>425</v>
+      </c>
+      <c r="E17" t="n">
+        <v>425</v>
+      </c>
+      <c r="H17" t="n">
+        <v>3</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>34800</v>
+      </c>
+      <c r="K17" t="n">
+        <v>25</v>
+      </c>
+      <c r="L17" t="n">
+        <v>-25</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>18Mar2021</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>BANKNIFTY2131834800CE</t>
+        </is>
+      </c>
+      <c r="P17" t="n">
+        <v>55245</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>10026141</v>
+      </c>
+      <c r="R17" t="n">
+        <v>290.15</v>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>2021-03-17 09:59:05</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>Entry</t>
+        </is>
+      </c>
+      <c r="U17" t="n">
+        <v>-7253.749999999999</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6" t="n">
+        <v>44272.42708333334</v>
+      </c>
+      <c r="B18" t="n">
+        <v>425</v>
+      </c>
+      <c r="C18" t="n">
+        <v>425</v>
+      </c>
+      <c r="D18" t="n">
+        <v>425</v>
+      </c>
+      <c r="E18" t="n">
+        <v>425</v>
+      </c>
+      <c r="H18" t="n">
+        <v>2</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>14850</v>
+      </c>
+      <c r="K18" t="n">
+        <v>75</v>
+      </c>
+      <c r="L18" t="n">
+        <v>-75</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>18Mar2021</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>NIFTY2131814850PE</t>
+        </is>
+      </c>
+      <c r="P18" t="n">
+        <v>56445</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>10026142</v>
+      </c>
+      <c r="R18" t="n">
+        <v>74.40000000000001</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>2021-03-17 09:59:05</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>Entry</t>
+        </is>
+      </c>
+      <c r="U18" t="n">
+        <v>-5580</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6" t="n">
+        <v>44272.42777777778</v>
+      </c>
+      <c r="B19" t="n">
+        <v>425</v>
+      </c>
+      <c r="C19" t="n">
+        <v>425</v>
+      </c>
+      <c r="D19" t="n">
+        <v>425</v>
+      </c>
+      <c r="E19" t="n">
+        <v>425</v>
+      </c>
+      <c r="H19" t="n">
+        <v>4</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>34600</v>
+      </c>
+      <c r="K19" t="n">
+        <v>25</v>
+      </c>
+      <c r="L19" t="n">
+        <v>-25</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>18Mar2021</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>BANKNIFTY2131834600PE</t>
+        </is>
+      </c>
+      <c r="P19" t="n">
+        <v>55197</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>10026143</v>
+      </c>
+      <c r="R19" t="n">
+        <v>295.35</v>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>2021-03-17 09:59:06</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>Entry</t>
+        </is>
+      </c>
+      <c r="U19" t="n">
+        <v>-7383.750000000001</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="6" t="n">
+        <v>44272.42847222222</v>
+      </c>
+      <c r="B20" t="n">
+        <v>425</v>
+      </c>
+      <c r="C20" t="n">
+        <v>425</v>
+      </c>
+      <c r="D20" t="n">
+        <v>263.75</v>
+      </c>
+      <c r="E20" t="n">
+        <v>263.75</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>sell</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>14950</v>
+      </c>
+      <c r="K20" t="n">
+        <v>75</v>
+      </c>
+      <c r="L20" t="n">
+        <v>-75</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>18Mar2021</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>NIFTY2131814950CE</t>
+        </is>
+      </c>
+      <c r="P20" t="n">
+        <v>56448</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>10026144</v>
+      </c>
+      <c r="R20" t="n">
+        <v>72.95</v>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>2021-03-17 09:59:06</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>Entry</t>
+        </is>
+      </c>
+      <c r="U20" t="n">
+        <v>-5471.25</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="6" t="n">
+        <v>44272.42916666667</v>
+      </c>
+      <c r="B21" t="n">
+        <v>263.75</v>
+      </c>
+      <c r="C21" t="n">
+        <v>368.75</v>
+      </c>
+      <c r="D21" t="n">
+        <v>263.75</v>
+      </c>
+      <c r="E21" t="n">
+        <v>368.75</v>
+      </c>
+      <c r="H21" t="n">
+        <v>3</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>34800</v>
+      </c>
+      <c r="K21" t="n">
+        <v>25</v>
+      </c>
+      <c r="L21" t="n">
+        <v>25</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>18Mar2021</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>BANKNIFTY2131834800CE</t>
+        </is>
+      </c>
+      <c r="P21" t="n">
+        <v>55245</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>10026145</v>
+      </c>
+      <c r="R21" t="n">
+        <v>351.85</v>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>2021-03-17 10:39:14</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>Repair</t>
+        </is>
+      </c>
+      <c r="U21" t="n">
+        <v>8796.25</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="6" t="n">
+        <v>44272.42986111111</v>
+      </c>
+      <c r="B22" t="n">
+        <v>368.75</v>
+      </c>
+      <c r="C22" t="n">
+        <v>368.75</v>
+      </c>
+      <c r="D22" t="n">
+        <v>368.75</v>
+      </c>
+      <c r="E22" t="n">
+        <v>368.75</v>
+      </c>
+      <c r="H22" t="n">
+        <v>2</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
+        <v>14850</v>
+      </c>
+      <c r="K22" t="n">
+        <v>75</v>
+      </c>
+      <c r="L22" t="n">
+        <v>75</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>18Mar2021</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>NIFTY2131814850PE</t>
+        </is>
+      </c>
+      <c r="P22" t="n">
+        <v>56445</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>10026146</v>
+      </c>
+      <c r="R22" t="n">
+        <v>89.95</v>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>2021-03-17 10:26:09</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>Repair</t>
+        </is>
+      </c>
+      <c r="U22" t="n">
+        <v>6746.25</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="6" t="n">
+        <v>44272.43055555555</v>
+      </c>
+      <c r="B23" t="n">
+        <v>368.75</v>
+      </c>
+      <c r="C23" t="n">
+        <v>626.25</v>
+      </c>
+      <c r="D23" t="n">
+        <v>368.75</v>
+      </c>
+      <c r="E23" t="n">
+        <v>495</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
+        <v>14950</v>
+      </c>
+      <c r="K23" t="n">
+        <v>75</v>
+      </c>
+      <c r="L23" t="n">
+        <v>75</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>18Mar2021</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>CE</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>NIFTY2131814950CE</t>
+        </is>
+      </c>
+      <c r="P23" t="n">
+        <v>56448</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>10026147</v>
+      </c>
+      <c r="R23" t="n">
+        <v>88.45</v>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>2021-03-17 11:31:19</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>Repair</t>
+        </is>
+      </c>
+      <c r="U23" t="n">
+        <v>6633.75</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="6" t="n">
+        <v>44272.43125</v>
+      </c>
+      <c r="B24" t="n">
+        <v>495</v>
+      </c>
+      <c r="C24" t="n">
+        <v>733.75</v>
+      </c>
+      <c r="D24" t="n">
+        <v>495</v>
+      </c>
+      <c r="E24" t="n">
+        <v>733.75</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="J24" t="n">
+        <v>34600</v>
+      </c>
+      <c r="K24" t="n">
+        <v>25</v>
+      </c>
+      <c r="L24" t="n">
+        <v>25</v>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>BANKNIFTY2131834600PE</t>
+        </is>
+      </c>
+      <c r="P24" t="n">
+        <v>55197</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>10026277</v>
+      </c>
+      <c r="R24" t="n">
+        <v>266</v>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>2021-03-17 12:40:35</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>Universal_Exit</t>
+        </is>
+      </c>
+      <c r="U24" t="n">
+        <v>6650</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="6" t="n">
+        <v>44272.43194444444</v>
+      </c>
+      <c r="B25" t="n">
+        <v>631.25</v>
+      </c>
+      <c r="C25" t="n">
+        <v>647.5</v>
+      </c>
+      <c r="D25" t="n">
+        <v>605</v>
+      </c>
+      <c r="E25" t="n">
+        <v>647.5</v>
+      </c>
+      <c r="H25" t="n">
+        <v>4</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>buy</t>
+        </is>
+      </c>
+      <c r="J25" t="n">
+        <v>34600</v>
+      </c>
+      <c r="K25" t="n">
+        <v>25</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>18Mar2021</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>PE</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>BANKNIFTY2131834600PE</t>
+        </is>
+      </c>
+      <c r="P25" t="n">
+        <v>55197</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>Repair</t>
+        </is>
+      </c>
+      <c r="U25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="n">
+        <v>44272.43263888889</v>
+      </c>
+      <c r="B26" t="n">
+        <v>680</v>
+      </c>
+      <c r="C26" t="n">
+        <v>682.5</v>
+      </c>
+      <c r="D26" t="n">
+        <v>598.75</v>
+      </c>
+      <c r="E26" t="n">
+        <v>598.75</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="n">
+        <v>44272.43333333333</v>
+      </c>
+      <c r="B27" t="n">
+        <v>628.75</v>
+      </c>
+      <c r="C27" t="n">
+        <v>628.75</v>
+      </c>
+      <c r="D27" t="n">
+        <v>521.25</v>
+      </c>
+      <c r="E27" t="n">
+        <v>521.25</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="n">
+        <v>44272.43402777778</v>
+      </c>
+      <c r="B28" t="n">
+        <v>587.5</v>
+      </c>
+      <c r="C28" t="n">
+        <v>587.5</v>
+      </c>
+      <c r="D28" t="n">
+        <v>332.5</v>
+      </c>
+      <c r="E28" t="n">
+        <v>332.5</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="n">
+        <v>44272.43472222222</v>
+      </c>
+      <c r="B29" t="n">
+        <v>450</v>
+      </c>
+      <c r="C29" t="n">
+        <v>450</v>
+      </c>
+      <c r="D29" t="n">
+        <v>311.25</v>
+      </c>
+      <c r="E29" t="n">
+        <v>318.75</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="n">
+        <v>44272.43541666667</v>
+      </c>
+      <c r="B30" t="n">
+        <v>320</v>
+      </c>
+      <c r="C30" t="n">
+        <v>433.75</v>
+      </c>
+      <c r="D30" t="n">
+        <v>293.75</v>
+      </c>
+      <c r="E30" t="n">
+        <v>293.75</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="n">
+        <v>44272.43611111111</v>
+      </c>
+      <c r="B31" t="n">
+        <v>318.75</v>
+      </c>
+      <c r="C31" t="n">
+        <v>457.5</v>
+      </c>
+      <c r="D31" t="n">
+        <v>275</v>
+      </c>
+      <c r="E31" t="n">
+        <v>452.5</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="n">
+        <v>44272.43680555555</v>
+      </c>
+      <c r="B32" t="n">
+        <v>452.5</v>
+      </c>
+      <c r="C32" t="n">
+        <v>600</v>
+      </c>
+      <c r="D32" t="n">
+        <v>452.5</v>
+      </c>
+      <c r="E32" t="n">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="n">
+        <v>44272.4375</v>
+      </c>
+      <c r="B33" t="n">
+        <v>672.5</v>
+      </c>
+      <c r="C33" t="n">
+        <v>728.75</v>
+      </c>
+      <c r="D33" t="n">
+        <v>588.75</v>
+      </c>
+      <c r="E33" t="n">
+        <v>718.75</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="n">
+        <v>44272.43819444445</v>
+      </c>
+      <c r="B34" t="n">
+        <v>877.5</v>
+      </c>
+      <c r="C34" t="n">
+        <v>997.5</v>
+      </c>
+      <c r="D34" t="n">
+        <v>791.25</v>
+      </c>
+      <c r="E34" t="n">
+        <v>791.25</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="n">
+        <v>44272.43888888889</v>
+      </c>
+      <c r="B35" t="n">
+        <v>791.25</v>
+      </c>
+      <c r="C35" t="n">
+        <v>805</v>
+      </c>
+      <c r="D35" t="n">
+        <v>733.75</v>
+      </c>
+      <c r="E35" t="n">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="6" t="n">
+        <v>44272.43958333333</v>
+      </c>
+      <c r="B36" t="n">
+        <v>805</v>
+      </c>
+      <c r="C36" t="n">
+        <v>847.5</v>
+      </c>
+      <c r="D36" t="n">
+        <v>772.5</v>
+      </c>
+      <c r="E36" t="n">
+        <v>772.5</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="n">
+        <v>44272.44027777778</v>
+      </c>
+      <c r="B37" t="n">
+        <v>752.5</v>
+      </c>
+      <c r="C37" t="n">
+        <v>752.5</v>
+      </c>
+      <c r="D37" t="n">
+        <v>717.5</v>
+      </c>
+      <c r="E37" t="n">
+        <v>736.25</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6" t="n">
+        <v>44272.44097222222</v>
+      </c>
+      <c r="B38" t="n">
+        <v>736.25</v>
+      </c>
+      <c r="C38" t="n">
+        <v>741.25</v>
+      </c>
+      <c r="D38" t="n">
+        <v>605</v>
+      </c>
+      <c r="E38" t="n">
+        <v>658.75</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="6" t="n">
+        <v>44272.44166666667</v>
+      </c>
+      <c r="B39" t="n">
+        <v>703.75</v>
+      </c>
+      <c r="C39" t="n">
+        <v>810</v>
+      </c>
+      <c r="D39" t="n">
+        <v>703.75</v>
+      </c>
+      <c r="E39" t="n">
+        <v>757.5</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="6" t="n">
+        <v>44272.44236111111</v>
+      </c>
+      <c r="B40" t="n">
+        <v>807.5</v>
+      </c>
+      <c r="C40" t="n">
+        <v>807.5</v>
+      </c>
+      <c r="D40" t="n">
+        <v>646.25</v>
+      </c>
+      <c r="E40" t="n">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="6" t="n">
+        <v>44272.44305555556</v>
+      </c>
+      <c r="B41" t="n">
+        <v>777.5</v>
+      </c>
+      <c r="C41" t="n">
+        <v>886.25</v>
+      </c>
+      <c r="D41" t="n">
+        <v>688.75</v>
+      </c>
+      <c r="E41" t="n">
+        <v>692.5</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="6" t="n">
+        <v>44272.44375</v>
+      </c>
+      <c r="B42" t="n">
+        <v>732.5</v>
+      </c>
+      <c r="C42" t="n">
+        <v>732.5</v>
+      </c>
+      <c r="D42" t="n">
+        <v>732.5</v>
+      </c>
+      <c r="E42" t="n">
+        <v>732.5</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="6" t="n">
+        <v>44272.44444444445</v>
+      </c>
+      <c r="B43" t="n">
+        <v>732.5</v>
+      </c>
+      <c r="C43" t="n">
+        <v>752.5</v>
+      </c>
+      <c r="D43" t="n">
+        <v>340</v>
+      </c>
+      <c r="E43" t="n">
+        <v>596.25</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="6" t="n">
+        <v>44272.44513888889</v>
+      </c>
+      <c r="B44" t="n">
+        <v>596.25</v>
+      </c>
+      <c r="C44" t="n">
+        <v>596.25</v>
+      </c>
+      <c r="D44" t="n">
+        <v>362.5</v>
+      </c>
+      <c r="E44" t="n">
+        <v>362.5</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="6" t="n">
+        <v>44272.44583333333</v>
+      </c>
+      <c r="B45" t="n">
+        <v>411.25</v>
+      </c>
+      <c r="C45" t="n">
+        <v>440</v>
+      </c>
+      <c r="D45" t="n">
+        <v>233.75</v>
+      </c>
+      <c r="E45" t="n">
+        <v>378.75</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="6" t="n">
+        <v>44272.44652777778</v>
+      </c>
+      <c r="B46" t="n">
+        <v>405</v>
+      </c>
+      <c r="C46" t="n">
+        <v>531.25</v>
+      </c>
+      <c r="D46" t="n">
+        <v>307.5</v>
+      </c>
+      <c r="E46" t="n">
+        <v>377.5</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="6" t="n">
+        <v>44272.44722222222</v>
+      </c>
+      <c r="B47" t="n">
+        <v>216.25</v>
+      </c>
+      <c r="C47" t="n">
+        <v>216.25</v>
+      </c>
+      <c r="D47" t="n">
+        <v>106.25</v>
+      </c>
+      <c r="E47" t="n">
+        <v>106.25</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="6" t="n">
+        <v>44272.44791666666</v>
+      </c>
+      <c r="B48" t="n">
+        <v>91.25</v>
+      </c>
+      <c r="C48" t="n">
+        <v>153.75</v>
+      </c>
+      <c r="D48" t="n">
+        <v>-35</v>
+      </c>
+      <c r="E48" t="n">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="6" t="n">
+        <v>44272.44861111111</v>
+      </c>
+      <c r="B49" t="n">
+        <v>21.25</v>
+      </c>
+      <c r="C49" t="n">
+        <v>21.25</v>
+      </c>
+      <c r="D49" t="n">
+        <v>-203.75</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-203.75</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="6" t="n">
+        <v>44272.44930555556</v>
+      </c>
+      <c r="B50" t="n">
+        <v>-25</v>
+      </c>
+      <c r="C50" t="n">
+        <v>73.75</v>
+      </c>
+      <c r="D50" t="n">
+        <v>-146.25</v>
+      </c>
+      <c r="E50" t="n">
+        <v>73.75</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="6" t="n">
+        <v>44272.45</v>
+      </c>
+      <c r="B51" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="C51" t="n">
+        <v>112.5</v>
+      </c>
+      <c r="D51" t="n">
+        <v>-62.5</v>
+      </c>
+      <c r="E51" t="n">
+        <v>-6.25</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="6" t="n">
+        <v>44272.45069444444</v>
+      </c>
+      <c r="B52" t="n">
+        <v>132.5</v>
+      </c>
+      <c r="C52" t="n">
+        <v>132.5</v>
+      </c>
+      <c r="D52" t="n">
+        <v>132.5</v>
+      </c>
+      <c r="E52" t="n">
+        <v>132.5</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="6" t="n">
+        <v>44272.45138888889</v>
+      </c>
+      <c r="B53" t="n">
+        <v>132.5</v>
+      </c>
+      <c r="C53" t="n">
+        <v>132.5</v>
+      </c>
+      <c r="D53" t="n">
+        <v>132.5</v>
+      </c>
+      <c r="E53" t="n">
+        <v>132.5</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="6" t="n">
+        <v>44272.45208333333</v>
+      </c>
+      <c r="B54" t="n">
+        <v>132.5</v>
+      </c>
+      <c r="C54" t="n">
+        <v>276.25</v>
+      </c>
+      <c r="D54" t="n">
+        <v>96.25</v>
+      </c>
+      <c r="E54" t="n">
+        <v>128.75</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="6" t="n">
+        <v>44272.45277777778</v>
+      </c>
+      <c r="B55" t="n">
+        <v>172.5</v>
+      </c>
+      <c r="C55" t="n">
+        <v>266.25</v>
+      </c>
+      <c r="D55" t="n">
+        <v>172.5</v>
+      </c>
+      <c r="E55" t="n">
+        <v>266.25</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="6" t="n">
+        <v>44272.45347222222</v>
+      </c>
+      <c r="B56" t="n">
+        <v>266.25</v>
+      </c>
+      <c r="C56" t="n">
+        <v>363.75</v>
+      </c>
+      <c r="D56" t="n">
+        <v>266.25</v>
+      </c>
+      <c r="E56" t="n">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="6" t="n">
+        <v>44272.45416666667</v>
+      </c>
+      <c r="B57" t="n">
+        <v>360</v>
+      </c>
+      <c r="C57" t="n">
+        <v>535</v>
+      </c>
+      <c r="D57" t="n">
+        <v>360</v>
+      </c>
+      <c r="E57" t="n">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="6" t="n">
+        <v>44272.45486111111</v>
+      </c>
+      <c r="B58" t="n">
+        <v>485</v>
+      </c>
+      <c r="C58" t="n">
+        <v>522.5</v>
+      </c>
+      <c r="D58" t="n">
+        <v>400</v>
+      </c>
+      <c r="E58" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="6" t="n">
+        <v>44272.45555555556</v>
+      </c>
+      <c r="B59" t="n">
+        <v>350</v>
+      </c>
+      <c r="C59" t="n">
+        <v>350</v>
+      </c>
+      <c r="D59" t="n">
+        <v>137.5</v>
+      </c>
+      <c r="E59" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="6" t="n">
+        <v>44272.45625</v>
+      </c>
+      <c r="B60" t="n">
+        <v>113.75</v>
+      </c>
+      <c r="C60" t="n">
+        <v>113.75</v>
+      </c>
+      <c r="D60" t="n">
+        <v>113.75</v>
+      </c>
+      <c r="E60" t="n">
+        <v>113.75</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="6" t="n">
+        <v>44272.45694444444</v>
+      </c>
+      <c r="B61" t="n">
+        <v>113.75</v>
+      </c>
+      <c r="C61" t="n">
+        <v>113.75</v>
+      </c>
+      <c r="D61" t="n">
+        <v>113.75</v>
+      </c>
+      <c r="E61" t="n">
+        <v>113.75</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="6" t="n">
+        <v>44272.45763888889</v>
+      </c>
+      <c r="B62" t="n">
+        <v>113.75</v>
+      </c>
+      <c r="C62" t="n">
+        <v>113.75</v>
+      </c>
+      <c r="D62" t="n">
+        <v>113.75</v>
+      </c>
+      <c r="E62" t="n">
+        <v>113.75</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="6" t="n">
+        <v>44272.45833333334</v>
+      </c>
+      <c r="B63" t="n">
+        <v>113.75</v>
+      </c>
+      <c r="C63" t="n">
+        <v>113.75</v>
+      </c>
+      <c r="D63" t="n">
+        <v>113.75</v>
+      </c>
+      <c r="E63" t="n">
+        <v>113.75</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="6" t="n">
+        <v>44272.45902777778</v>
+      </c>
+      <c r="B64" t="n">
+        <v>113.75</v>
+      </c>
+      <c r="C64" t="n">
+        <v>297.5</v>
+      </c>
+      <c r="D64" t="n">
+        <v>113.75</v>
+      </c>
+      <c r="E64" t="n">
+        <v>297.5</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="6" t="n">
+        <v>44272.45972222222</v>
+      </c>
+      <c r="B65" t="n">
+        <v>297.5</v>
+      </c>
+      <c r="C65" t="n">
+        <v>297.5</v>
+      </c>
+      <c r="D65" t="n">
+        <v>297.5</v>
+      </c>
+      <c r="E65" t="n">
+        <v>297.5</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="6" t="n">
+        <v>44272.46041666667</v>
+      </c>
+      <c r="B66" t="n">
+        <v>297.5</v>
+      </c>
+      <c r="C66" t="n">
+        <v>297.5</v>
+      </c>
+      <c r="D66" t="n">
+        <v>111.25</v>
+      </c>
+      <c r="E66" t="n">
+        <v>111.25</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="6" t="n">
+        <v>44272.46111111111</v>
+      </c>
+      <c r="B67" t="n">
+        <v>111.25</v>
+      </c>
+      <c r="C67" t="n">
+        <v>111.25</v>
+      </c>
+      <c r="D67" t="n">
+        <v>-58.75</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-58.75</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="6" t="n">
+        <v>44272.46180555555</v>
+      </c>
+      <c r="B68" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="C68" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="D68" t="n">
+        <v>-90</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="6" t="n">
+        <v>44272.4625</v>
+      </c>
+      <c r="B69" t="n">
+        <v>-105</v>
+      </c>
+      <c r="C69" t="n">
+        <v>103.75</v>
+      </c>
+      <c r="D69" t="n">
+        <v>-105</v>
+      </c>
+      <c r="E69" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="6" t="n">
+        <v>44272.46319444444</v>
+      </c>
+      <c r="B70" t="n">
+        <v>-120</v>
+      </c>
+      <c r="C70" t="n">
+        <v>-82.5</v>
+      </c>
+      <c r="D70" t="n">
+        <v>-126.25</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-93.75</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="6" t="n">
+        <v>44272.46388888889</v>
+      </c>
+      <c r="B71" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="C71" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="D71" t="n">
+        <v>-133.75</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="6" t="n">
+        <v>44272.46458333333</v>
+      </c>
+      <c r="B72" t="n">
+        <v>45</v>
+      </c>
+      <c r="C72" t="n">
+        <v>45</v>
+      </c>
+      <c r="D72" t="n">
+        <v>-73.75</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-23.75</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="6" t="n">
+        <v>44272.46527777778</v>
+      </c>
+      <c r="B73" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="C73" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="D73" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="E73" t="n">
+        <v>-61.25</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="6" t="n">
+        <v>44272.46597222222</v>
+      </c>
+      <c r="B74" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="C74" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="D74" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-61.25</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="6" t="n">
+        <v>44272.46666666667</v>
+      </c>
+      <c r="B75" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="C75" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="D75" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-61.25</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="6" t="n">
+        <v>44272.46736111111</v>
+      </c>
+      <c r="B76" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="C76" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="D76" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-61.25</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="6" t="n">
+        <v>44272.46805555555</v>
+      </c>
+      <c r="B77" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="C77" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="D77" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="E77" t="n">
+        <v>-61.25</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="6" t="n">
+        <v>44272.46875</v>
+      </c>
+      <c r="B78" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="C78" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="D78" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-61.25</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="6" t="n">
+        <v>44272.46944444445</v>
+      </c>
+      <c r="B79" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="C79" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="D79" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-61.25</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="6" t="n">
+        <v>44272.47013888889</v>
+      </c>
+      <c r="B80" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="C80" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="D80" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-61.25</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="6" t="n">
+        <v>44272.47083333333</v>
+      </c>
+      <c r="B81" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="C81" t="n">
+        <v>952.5</v>
+      </c>
+      <c r="D81" t="n">
+        <v>-61.25</v>
+      </c>
+      <c r="E81" t="n">
+        <v>846.25</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="6" t="n">
+        <v>44272.47152777778</v>
+      </c>
+      <c r="B82" t="n">
+        <v>782.5</v>
+      </c>
+      <c r="C82" t="n">
+        <v>782.5</v>
+      </c>
+      <c r="D82" t="n">
+        <v>727.5</v>
+      </c>
+      <c r="E82" t="n">
+        <v>727.5</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="6" t="n">
+        <v>44272.47222222222</v>
+      </c>
+      <c r="B83" t="n">
+        <v>1088.75</v>
+      </c>
+      <c r="C83" t="n">
+        <v>1820</v>
+      </c>
+      <c r="D83" t="n">
+        <v>1088.75</v>
+      </c>
+      <c r="E83" t="n">
+        <v>1743.75</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="6" t="n">
+        <v>44272.47291666667</v>
+      </c>
+      <c r="B84" t="n">
+        <v>1756.25</v>
+      </c>
+      <c r="C84" t="n">
+        <v>2037.5</v>
+      </c>
+      <c r="D84" t="n">
+        <v>1756.25</v>
+      </c>
+      <c r="E84" t="n">
+        <v>2037.5</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="6" t="n">
+        <v>44272.47361111111</v>
+      </c>
+      <c r="B85" t="n">
+        <v>2037.5</v>
+      </c>
+      <c r="C85" t="n">
+        <v>2037.5</v>
+      </c>
+      <c r="D85" t="n">
+        <v>2037.5</v>
+      </c>
+      <c r="E85" t="n">
+        <v>2037.5</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="6" t="n">
+        <v>44272.47430555556</v>
+      </c>
+      <c r="B86" t="n">
+        <v>2037.5</v>
+      </c>
+      <c r="C86" t="n">
+        <v>2037.5</v>
+      </c>
+      <c r="D86" t="n">
+        <v>286.25</v>
+      </c>
+      <c r="E86" t="n">
+        <v>286.25</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="6" t="n">
+        <v>44272.475</v>
+      </c>
+      <c r="B87" t="n">
+        <v>286.25</v>
+      </c>
+      <c r="C87" t="n">
+        <v>286.25</v>
+      </c>
+      <c r="D87" t="n">
+        <v>286.25</v>
+      </c>
+      <c r="E87" t="n">
+        <v>286.25</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="6" t="n">
+        <v>44272.47569444445</v>
+      </c>
+      <c r="B88" t="n">
+        <v>286.25</v>
+      </c>
+      <c r="C88" t="n">
+        <v>286.25</v>
+      </c>
+      <c r="D88" t="n">
+        <v>253.75</v>
+      </c>
+      <c r="E88" t="n">
+        <v>253.75</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="6" t="n">
+        <v>44272.47638888889</v>
+      </c>
+      <c r="B89" t="n">
+        <v>225</v>
+      </c>
+      <c r="C89" t="n">
+        <v>326.25</v>
+      </c>
+      <c r="D89" t="n">
+        <v>167.5</v>
+      </c>
+      <c r="E89" t="n">
+        <v>286.25</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="6" t="n">
+        <v>44272.47708333333</v>
+      </c>
+      <c r="B90" t="n">
+        <v>298.75</v>
+      </c>
+      <c r="C90" t="n">
+        <v>315</v>
+      </c>
+      <c r="D90" t="n">
+        <v>165</v>
+      </c>
+      <c r="E90" t="n">
+        <v>272.5</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="6" t="n">
+        <v>44272.47777777778</v>
+      </c>
+      <c r="B91" t="n">
+        <v>247.5</v>
+      </c>
+      <c r="C91" t="n">
+        <v>273.75</v>
+      </c>
+      <c r="D91" t="n">
+        <v>175</v>
+      </c>
+      <c r="E91" t="n">
+        <v>176.25</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="6" t="n">
+        <v>44272.47847222222</v>
+      </c>
+      <c r="B92" t="n">
+        <v>213.75</v>
+      </c>
+      <c r="C92" t="n">
+        <v>575</v>
+      </c>
+      <c r="D92" t="n">
+        <v>187.5</v>
+      </c>
+      <c r="E92" t="n">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="6" t="n">
+        <v>44272.47916666666</v>
+      </c>
+      <c r="B93" t="n">
+        <v>686.25</v>
+      </c>
+      <c r="C93" t="n">
+        <v>900</v>
+      </c>
+      <c r="D93" t="n">
+        <v>686.25</v>
+      </c>
+      <c r="E93" t="n">
+        <v>716.25</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="6" t="n">
+        <v>44272.47986111111</v>
+      </c>
+      <c r="B94" t="n">
+        <v>668.75</v>
+      </c>
+      <c r="C94" t="n">
+        <v>668.75</v>
+      </c>
+      <c r="D94" t="n">
+        <v>161.25</v>
+      </c>
+      <c r="E94" t="n">
+        <v>161.25</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="6" t="n">
+        <v>44272.48055555556</v>
+      </c>
+      <c r="B95" t="n">
+        <v>102.5</v>
+      </c>
+      <c r="C95" t="n">
+        <v>168.75</v>
+      </c>
+      <c r="D95" t="n">
+        <v>92.5</v>
+      </c>
+      <c r="E95" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="6" t="n">
+        <v>44272.48125</v>
+      </c>
+      <c r="B96" t="n">
+        <v>120</v>
+      </c>
+      <c r="C96" t="n">
+        <v>120</v>
+      </c>
+      <c r="D96" t="n">
+        <v>16.25</v>
+      </c>
+      <c r="E96" t="n">
+        <v>16.25</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="6" t="n">
+        <v>44272.48194444444</v>
+      </c>
+      <c r="B97" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="C97" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="D97" t="n">
+        <v>-96.25</v>
+      </c>
+      <c r="E97" t="n">
+        <v>-96.25</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="6" t="n">
+        <v>44272.48263888889</v>
+      </c>
+      <c r="B98" t="n">
+        <v>-163.75</v>
+      </c>
+      <c r="C98" t="n">
+        <v>-163.75</v>
+      </c>
+      <c r="D98" t="n">
+        <v>-381.25</v>
+      </c>
+      <c r="E98" t="n">
+        <v>-337.5</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="6" t="n">
+        <v>44272.48333333333</v>
+      </c>
+      <c r="B99" t="n">
+        <v>-437.5</v>
+      </c>
+      <c r="C99" t="n">
+        <v>-252.5</v>
+      </c>
+      <c r="D99" t="n">
+        <v>-437.5</v>
+      </c>
+      <c r="E99" t="n">
+        <v>-333.75</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="6" t="n">
+        <v>44272.48402777778</v>
+      </c>
+      <c r="B100" t="n">
+        <v>-235</v>
+      </c>
+      <c r="C100" t="n">
+        <v>-97.5</v>
+      </c>
+      <c r="D100" t="n">
+        <v>-235</v>
+      </c>
+      <c r="E100" t="n">
+        <v>-156.25</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="6" t="n">
+        <v>44272.48472222222</v>
+      </c>
+      <c r="B101" t="n">
+        <v>-188.75</v>
+      </c>
+      <c r="C101" t="n">
+        <v>-173.75</v>
+      </c>
+      <c r="D101" t="n">
+        <v>-341.25</v>
+      </c>
+      <c r="E101" t="n">
+        <v>-341.25</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="6" t="n">
+        <v>44272.48541666667</v>
+      </c>
+      <c r="B102" t="n">
+        <v>-397.5</v>
+      </c>
+      <c r="C102" t="n">
+        <v>-300</v>
+      </c>
+      <c r="D102" t="n">
+        <v>-446.25</v>
+      </c>
+      <c r="E102" t="n">
+        <v>-446.25</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="6" t="n">
+        <v>44272.48611111111</v>
+      </c>
+      <c r="B103" t="n">
+        <v>-455</v>
+      </c>
+      <c r="C103" t="n">
+        <v>-395</v>
+      </c>
+      <c r="D103" t="n">
+        <v>-537.5</v>
+      </c>
+      <c r="E103" t="n">
+        <v>-395</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="6" t="n">
+        <v>44272.48680555556</v>
+      </c>
+      <c r="B104" t="n">
+        <v>-406.25</v>
+      </c>
+      <c r="C104" t="n">
+        <v>-281.25</v>
+      </c>
+      <c r="D104" t="n">
+        <v>-410</v>
+      </c>
+      <c r="E104" t="n">
+        <v>-360</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="6" t="n">
+        <v>44272.4875</v>
+      </c>
+      <c r="B105" t="n">
+        <v>-418.75</v>
+      </c>
+      <c r="C105" t="n">
+        <v>-395</v>
+      </c>
+      <c r="D105" t="n">
+        <v>-532.5</v>
+      </c>
+      <c r="E105" t="n">
+        <v>-532.5</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="6" t="n">
+        <v>44272.48819444444</v>
+      </c>
+      <c r="B106" t="n">
+        <v>-503.75</v>
+      </c>
+      <c r="C106" t="n">
+        <v>-462.5</v>
+      </c>
+      <c r="D106" t="n">
+        <v>-531.25</v>
+      </c>
+      <c r="E106" t="n">
+        <v>-530</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="6" t="n">
+        <v>44272.48888888889</v>
+      </c>
+      <c r="B107" t="n">
+        <v>-468.75</v>
+      </c>
+      <c r="C107" t="n">
+        <v>-391.25</v>
+      </c>
+      <c r="D107" t="n">
+        <v>-468.75</v>
+      </c>
+      <c r="E107" t="n">
+        <v>-465</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="6" t="n">
+        <v>44272.48958333334</v>
+      </c>
+      <c r="B108" t="n">
+        <v>-472.5</v>
+      </c>
+      <c r="C108" t="n">
+        <v>-445</v>
+      </c>
+      <c r="D108" t="n">
+        <v>-522.5</v>
+      </c>
+      <c r="E108" t="n">
+        <v>-463.75</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="6" t="n">
+        <v>44272.49027777778</v>
+      </c>
+      <c r="B109" t="n">
+        <v>-395</v>
+      </c>
+      <c r="C109" t="n">
+        <v>-223.75</v>
+      </c>
+      <c r="D109" t="n">
+        <v>-395</v>
+      </c>
+      <c r="E109" t="n">
+        <v>-273.75</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="6" t="n">
+        <v>44272.49097222222</v>
+      </c>
+      <c r="B110" t="n">
+        <v>-272.5</v>
+      </c>
+      <c r="C110" t="n">
+        <v>-260</v>
+      </c>
+      <c r="D110" t="n">
+        <v>-326.25</v>
+      </c>
+      <c r="E110" t="n">
+        <v>-260</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="6" t="n">
+        <v>44272.49166666667</v>
+      </c>
+      <c r="B111" t="n">
+        <v>-93.75</v>
+      </c>
+      <c r="C111" t="n">
+        <v>-93.75</v>
+      </c>
+      <c r="D111" t="n">
+        <v>-251.25</v>
+      </c>
+      <c r="E111" t="n">
+        <v>-205</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="6" t="n">
+        <v>44272.49236111111</v>
+      </c>
+      <c r="B112" t="n">
+        <v>-231.25</v>
+      </c>
+      <c r="C112" t="n">
+        <v>-231.25</v>
+      </c>
+      <c r="D112" t="n">
+        <v>-346.25</v>
+      </c>
+      <c r="E112" t="n">
+        <v>-346.25</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="6" t="n">
+        <v>44272.49305555555</v>
+      </c>
+      <c r="B113" t="n">
+        <v>-350</v>
+      </c>
+      <c r="C113" t="n">
+        <v>-350</v>
+      </c>
+      <c r="D113" t="n">
+        <v>-537.5</v>
+      </c>
+      <c r="E113" t="n">
+        <v>-537.5</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="6" t="n">
+        <v>44272.49375</v>
+      </c>
+      <c r="B114" t="n">
+        <v>-497.5</v>
+      </c>
+      <c r="C114" t="n">
+        <v>-497.5</v>
+      </c>
+      <c r="D114" t="n">
+        <v>-701.25</v>
+      </c>
+      <c r="E114" t="n">
+        <v>-701.25</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="6" t="n">
+        <v>44272.49444444444</v>
+      </c>
+      <c r="B115" t="n">
+        <v>-637.5</v>
+      </c>
+      <c r="C115" t="n">
+        <v>-637.5</v>
+      </c>
+      <c r="D115" t="n">
+        <v>-702.5</v>
+      </c>
+      <c r="E115" t="n">
+        <v>-702.5</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="6" t="n">
+        <v>44272.49513888889</v>
+      </c>
+      <c r="B116" t="n">
+        <v>-655</v>
+      </c>
+      <c r="C116" t="n">
+        <v>-616.25</v>
+      </c>
+      <c r="D116" t="n">
+        <v>-720</v>
+      </c>
+      <c r="E116" t="n">
+        <v>-720</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="6" t="n">
+        <v>44272.49583333333</v>
+      </c>
+      <c r="B117" t="n">
+        <v>-692.5</v>
+      </c>
+      <c r="C117" t="n">
+        <v>-692.5</v>
+      </c>
+      <c r="D117" t="n">
+        <v>-791.25</v>
+      </c>
+      <c r="E117" t="n">
+        <v>-762.5</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="6" t="n">
+        <v>44272.49652777778</v>
+      </c>
+      <c r="B118" t="n">
+        <v>-882.5</v>
+      </c>
+      <c r="C118" t="n">
+        <v>-655</v>
+      </c>
+      <c r="D118" t="n">
+        <v>-882.5</v>
+      </c>
+      <c r="E118" t="n">
+        <v>-686.25</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="6" t="n">
+        <v>44272.49722222222</v>
+      </c>
+      <c r="B119" t="n">
+        <v>-690</v>
+      </c>
+      <c r="C119" t="n">
+        <v>-641.25</v>
+      </c>
+      <c r="D119" t="n">
+        <v>-755</v>
+      </c>
+      <c r="E119" t="n">
+        <v>-755</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="6" t="n">
+        <v>44272.49791666667</v>
+      </c>
+      <c r="B120" t="n">
+        <v>-826.25</v>
+      </c>
+      <c r="C120" t="n">
+        <v>-757.5</v>
+      </c>
+      <c r="D120" t="n">
+        <v>-873.75</v>
+      </c>
+      <c r="E120" t="n">
+        <v>-765</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="6" t="n">
+        <v>44272.49861111111</v>
+      </c>
+      <c r="B121" t="n">
+        <v>-750</v>
+      </c>
+      <c r="C121" t="n">
+        <v>-716.25</v>
+      </c>
+      <c r="D121" t="n">
+        <v>-1018.75</v>
+      </c>
+      <c r="E121" t="n">
+        <v>-1018.75</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="6" t="n">
+        <v>44272.49930555555</v>
+      </c>
+      <c r="B122" t="n">
+        <v>-932.5</v>
+      </c>
+      <c r="C122" t="n">
+        <v>-926.25</v>
+      </c>
+      <c r="D122" t="n">
+        <v>-1080</v>
+      </c>
+      <c r="E122" t="n">
+        <v>-1080</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="6" t="n">
+        <v>44272.5</v>
+      </c>
+      <c r="B123" t="n">
+        <v>-1041.25</v>
+      </c>
+      <c r="C123" t="n">
+        <v>-967.5</v>
+      </c>
+      <c r="D123" t="n">
+        <v>-1077.5</v>
+      </c>
+      <c r="E123" t="n">
+        <v>-982.5</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="6" t="n">
+        <v>44272.50069444445</v>
+      </c>
+      <c r="B124" t="n">
+        <v>-866.25</v>
+      </c>
+      <c r="C124" t="n">
+        <v>-798.75</v>
+      </c>
+      <c r="D124" t="n">
+        <v>-866.25</v>
+      </c>
+      <c r="E124" t="n">
+        <v>-856.25</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="6" t="n">
+        <v>44272.50138888889</v>
+      </c>
+      <c r="B125" t="n">
+        <v>-845</v>
+      </c>
+      <c r="C125" t="n">
+        <v>-770</v>
+      </c>
+      <c r="D125" t="n">
+        <v>-916.25</v>
+      </c>
+      <c r="E125" t="n">
+        <v>-916.25</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="6" t="n">
+        <v>44272.50208333333</v>
+      </c>
+      <c r="B126" t="n">
+        <v>-912.5</v>
+      </c>
+      <c r="C126" t="n">
+        <v>-912.5</v>
+      </c>
+      <c r="D126" t="n">
+        <v>-1312.5</v>
+      </c>
+      <c r="E126" t="n">
+        <v>-1312.5</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="6" t="n">
+        <v>44272.50277777778</v>
+      </c>
+      <c r="B127" t="n">
+        <v>-1396.25</v>
+      </c>
+      <c r="C127" t="n">
+        <v>-1225</v>
+      </c>
+      <c r="D127" t="n">
+        <v>-1396.25</v>
+      </c>
+      <c r="E127" t="n">
+        <v>-1316.25</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="6" t="n">
+        <v>44272.50347222222</v>
+      </c>
+      <c r="B128" t="n">
+        <v>-1387.5</v>
+      </c>
+      <c r="C128" t="n">
+        <v>-1387.5</v>
+      </c>
+      <c r="D128" t="n">
+        <v>-1575</v>
+      </c>
+      <c r="E128" t="n">
+        <v>-1411.25</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="6" t="n">
+        <v>44272.50416666667</v>
+      </c>
+      <c r="B129" t="n">
+        <v>-1503.75</v>
+      </c>
+      <c r="C129" t="n">
+        <v>-1423.75</v>
+      </c>
+      <c r="D129" t="n">
+        <v>-1503.75</v>
+      </c>
+      <c r="E129" t="n">
+        <v>-1471.25</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="6" t="n">
+        <v>44272.50486111111</v>
+      </c>
+      <c r="B130" t="n">
+        <v>-1602.5</v>
+      </c>
+      <c r="C130" t="n">
+        <v>-1503.75</v>
+      </c>
+      <c r="D130" t="n">
+        <v>-2053.75</v>
+      </c>
+      <c r="E130" t="n">
+        <v>-2053.75</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="6" t="n">
+        <v>44272.50555555556</v>
+      </c>
+      <c r="B131" t="n">
+        <v>-2403.75</v>
+      </c>
+      <c r="C131" t="n">
+        <v>-1833.75</v>
+      </c>
+      <c r="D131" t="n">
+        <v>-2403.75</v>
+      </c>
+      <c r="E131" t="n">
+        <v>-1833.75</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="6" t="n">
+        <v>44272.50625</v>
+      </c>
+      <c r="B132" t="n">
+        <v>-1811.25</v>
+      </c>
+      <c r="C132" t="n">
+        <v>-1811.25</v>
+      </c>
+      <c r="D132" t="n">
+        <v>-2035</v>
+      </c>
+      <c r="E132" t="n">
+        <v>-1895</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="6" t="n">
+        <v>44272.50694444445</v>
+      </c>
+      <c r="B133" t="n">
+        <v>-1970</v>
+      </c>
+      <c r="C133" t="n">
+        <v>-1803.75</v>
+      </c>
+      <c r="D133" t="n">
+        <v>-2025</v>
+      </c>
+      <c r="E133" t="n">
+        <v>-1895</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="6" t="n">
+        <v>44272.50763888889</v>
+      </c>
+      <c r="B134" t="n">
+        <v>-1972.5</v>
+      </c>
+      <c r="C134" t="n">
+        <v>-1540</v>
+      </c>
+      <c r="D134" t="n">
+        <v>-2033.75</v>
+      </c>
+      <c r="E134" t="n">
+        <v>-1540</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="6" t="n">
+        <v>44272.50833333333</v>
+      </c>
+      <c r="B135" t="n">
+        <v>-1707.5</v>
+      </c>
+      <c r="C135" t="n">
+        <v>-1685</v>
+      </c>
+      <c r="D135" t="n">
+        <v>-1875</v>
+      </c>
+      <c r="E135" t="n">
+        <v>-1783.75</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="6" t="n">
+        <v>44272.50902777778</v>
+      </c>
+      <c r="B136" t="n">
+        <v>-1856.25</v>
+      </c>
+      <c r="C136" t="n">
+        <v>-1856.25</v>
+      </c>
+      <c r="D136" t="n">
+        <v>-2076.25</v>
+      </c>
+      <c r="E136" t="n">
+        <v>-2022.5</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="6" t="n">
+        <v>44272.50972222222</v>
+      </c>
+      <c r="B137" t="n">
+        <v>-1915</v>
+      </c>
+      <c r="C137" t="n">
+        <v>-1812.5</v>
+      </c>
+      <c r="D137" t="n">
+        <v>-2030</v>
+      </c>
+      <c r="E137" t="n">
+        <v>-1812.5</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="6" t="n">
+        <v>44272.51041666666</v>
+      </c>
+      <c r="B138" t="n">
+        <v>-1848.75</v>
+      </c>
+      <c r="C138" t="n">
+        <v>-1551.25</v>
+      </c>
+      <c r="D138" t="n">
+        <v>-1848.75</v>
+      </c>
+      <c r="E138" t="n">
+        <v>-1551.25</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="6" t="n">
+        <v>44272.51111111111</v>
+      </c>
+      <c r="B139" t="n">
+        <v>-1541.25</v>
+      </c>
+      <c r="C139" t="n">
+        <v>-1413.75</v>
+      </c>
+      <c r="D139" t="n">
+        <v>-1850</v>
+      </c>
+      <c r="E139" t="n">
+        <v>-1792.5</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="6" t="n">
+        <v>44272.51180555556</v>
+      </c>
+      <c r="B140" t="n">
+        <v>-1758.75</v>
+      </c>
+      <c r="C140" t="n">
+        <v>-1758.75</v>
+      </c>
+      <c r="D140" t="n">
+        <v>-2180</v>
+      </c>
+      <c r="E140" t="n">
+        <v>-2092.5</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="6" t="n">
+        <v>44272.5125</v>
+      </c>
+      <c r="B141" t="n">
+        <v>-2041.25</v>
+      </c>
+      <c r="C141" t="n">
+        <v>-2025</v>
+      </c>
+      <c r="D141" t="n">
+        <v>-2200</v>
+      </c>
+      <c r="E141" t="n">
+        <v>-2200</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="6" t="n">
+        <v>44272.51319444444</v>
+      </c>
+      <c r="B142" t="n">
+        <v>-2138.75</v>
+      </c>
+      <c r="C142" t="n">
+        <v>-2068.75</v>
+      </c>
+      <c r="D142" t="n">
+        <v>-2215</v>
+      </c>
+      <c r="E142" t="n">
+        <v>-2178.75</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="6" t="n">
+        <v>44272.51388888889</v>
+      </c>
+      <c r="B143" t="n">
+        <v>-2196.25</v>
+      </c>
+      <c r="C143" t="n">
+        <v>-1863.75</v>
+      </c>
+      <c r="D143" t="n">
+        <v>-2196.25</v>
+      </c>
+      <c r="E143" t="n">
+        <v>-1863.75</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="6" t="n">
+        <v>44272.51458333333</v>
+      </c>
+      <c r="B144" t="n">
+        <v>-1955</v>
+      </c>
+      <c r="C144" t="n">
+        <v>-1955</v>
+      </c>
+      <c r="D144" t="n">
+        <v>-2492.5</v>
+      </c>
+      <c r="E144" t="n">
+        <v>-2492.5</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="6" t="n">
+        <v>44272.51527777778</v>
+      </c>
+      <c r="B145" t="n">
+        <v>-2721.25</v>
+      </c>
+      <c r="C145" t="n">
+        <v>-2358.75</v>
+      </c>
+      <c r="D145" t="n">
+        <v>-2721.25</v>
+      </c>
+      <c r="E145" t="n">
+        <v>-2358.75</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="6" t="n">
+        <v>44272.51597222222</v>
+      </c>
+      <c r="B146" t="n">
+        <v>-2206.25</v>
+      </c>
+      <c r="C146" t="n">
+        <v>-2206.25</v>
+      </c>
+      <c r="D146" t="n">
+        <v>-2411.25</v>
+      </c>
+      <c r="E146" t="n">
+        <v>-2243.75</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="6" t="n">
+        <v>44272.51666666667</v>
+      </c>
+      <c r="B147" t="n">
+        <v>-2156.25</v>
+      </c>
+      <c r="C147" t="n">
+        <v>-2142.5</v>
+      </c>
+      <c r="D147" t="n">
+        <v>-2225</v>
+      </c>
+      <c r="E147" t="n">
+        <v>-2225</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="6" t="n">
+        <v>44272.51736111111</v>
+      </c>
+      <c r="B148" t="n">
+        <v>-2303.75</v>
+      </c>
+      <c r="C148" t="n">
+        <v>-2133.75</v>
+      </c>
+      <c r="D148" t="n">
+        <v>-2346.25</v>
+      </c>
+      <c r="E148" t="n">
+        <v>-2133.75</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="6" t="n">
+        <v>44272.51805555556</v>
+      </c>
+      <c r="B149" t="n">
+        <v>-1962.5</v>
+      </c>
+      <c r="C149" t="n">
+        <v>-1962.5</v>
+      </c>
+      <c r="D149" t="n">
+        <v>-2191.25</v>
+      </c>
+      <c r="E149" t="n">
+        <v>-2191.25</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="6" t="n">
+        <v>44272.51875</v>
+      </c>
+      <c r="B150" t="n">
+        <v>-2145</v>
+      </c>
+      <c r="C150" t="n">
+        <v>-1980</v>
+      </c>
+      <c r="D150" t="n">
+        <v>-2145</v>
+      </c>
+      <c r="E150" t="n">
+        <v>-2103.75</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="6" t="n">
+        <v>44272.51944444444</v>
+      </c>
+      <c r="B151" t="n">
+        <v>-2097.5</v>
+      </c>
+      <c r="C151" t="n">
+        <v>-2097.5</v>
+      </c>
+      <c r="D151" t="n">
+        <v>-2377.5</v>
+      </c>
+      <c r="E151" t="n">
+        <v>-2212.5</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="6" t="n">
+        <v>44272.52013888889</v>
+      </c>
+      <c r="B152" t="n">
+        <v>-2321.25</v>
+      </c>
+      <c r="C152" t="n">
+        <v>-2045</v>
+      </c>
+      <c r="D152" t="n">
+        <v>-2321.25</v>
+      </c>
+      <c r="E152" t="n">
+        <v>-2045</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="6" t="n">
+        <v>44272.52083333334</v>
+      </c>
+      <c r="B153" t="n">
+        <v>-1865</v>
+      </c>
+      <c r="C153" t="n">
+        <v>-1865</v>
+      </c>
+      <c r="D153" t="n">
+        <v>-2110</v>
+      </c>
+      <c r="E153" t="n">
+        <v>-2060</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="6" t="n">
+        <v>44272.52152777778</v>
+      </c>
+      <c r="B154" t="n">
+        <v>-2053.75</v>
+      </c>
+      <c r="C154" t="n">
+        <v>-2053.75</v>
+      </c>
+      <c r="D154" t="n">
+        <v>-2212.5</v>
+      </c>
+      <c r="E154" t="n">
+        <v>-2212.5</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="6" t="n">
+        <v>44272.52222222222</v>
+      </c>
+      <c r="B155" t="n">
+        <v>-2165</v>
+      </c>
+      <c r="C155" t="n">
+        <v>-1905</v>
+      </c>
+      <c r="D155" t="n">
+        <v>-2165</v>
+      </c>
+      <c r="E155" t="n">
+        <v>-1973.75</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="6" t="n">
+        <v>44272.52291666667</v>
+      </c>
+      <c r="B156" t="n">
+        <v>-1950</v>
+      </c>
+      <c r="C156" t="n">
+        <v>-1781.25</v>
+      </c>
+      <c r="D156" t="n">
+        <v>-2031.25</v>
+      </c>
+      <c r="E156" t="n">
+        <v>-2031.25</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="6" t="n">
+        <v>44272.52361111111</v>
+      </c>
+      <c r="B157" t="n">
+        <v>-2096.25</v>
+      </c>
+      <c r="C157" t="n">
+        <v>-2062.5</v>
+      </c>
+      <c r="D157" t="n">
+        <v>-2237.5</v>
+      </c>
+      <c r="E157" t="n">
+        <v>-2193.75</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="6" t="n">
+        <v>44272.52430555555</v>
+      </c>
+      <c r="B158" t="n">
+        <v>-2236.25</v>
+      </c>
+      <c r="C158" t="n">
+        <v>-2236.25</v>
+      </c>
+      <c r="D158" t="n">
+        <v>-2493.75</v>
+      </c>
+      <c r="E158" t="n">
+        <v>-2493.75</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="6" t="n">
+        <v>44272.525</v>
+      </c>
+      <c r="B159" t="n">
+        <v>-2503.75</v>
+      </c>
+      <c r="C159" t="n">
+        <v>-2503.75</v>
+      </c>
+      <c r="D159" t="n">
+        <v>-2798.75</v>
+      </c>
+      <c r="E159" t="n">
+        <v>-2732.5</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="6" t="n">
+        <v>44272.52569444444</v>
+      </c>
+      <c r="B160" t="n">
+        <v>-2876.25</v>
+      </c>
+      <c r="C160" t="n">
+        <v>-2876.25</v>
+      </c>
+      <c r="D160" t="n">
+        <v>-2957.5</v>
+      </c>
+      <c r="E160" t="n">
+        <v>-2915</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="6" t="n">
+        <v>44272.52638888889</v>
+      </c>
+      <c r="B161" t="n">
+        <v>-2826.25</v>
+      </c>
+      <c r="C161" t="n">
+        <v>-2695</v>
+      </c>
+      <c r="D161" t="n">
+        <v>-2918.75</v>
+      </c>
+      <c r="E161" t="n">
+        <v>-2695</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="6" t="n">
+        <v>44272.52708333333</v>
+      </c>
+      <c r="B162" t="n">
+        <v>-2800</v>
+      </c>
+      <c r="C162" t="n">
+        <v>-2626.25</v>
+      </c>
+      <c r="D162" t="n">
+        <v>-2802.5</v>
+      </c>
+      <c r="E162" t="n">
+        <v>-2768.75</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="6" t="n">
+        <v>44272.52777777778</v>
+      </c>
+      <c r="B163" t="n">
+        <v>-2936.25</v>
+      </c>
+      <c r="C163" t="n">
+        <v>-2906.25</v>
+      </c>
+      <c r="D163" t="n">
+        <v>-3137.5</v>
+      </c>
+      <c r="E163" t="n">
+        <v>-3137.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>